<commit_message>
Initial working Bar chart with hardcoded values.
</commit_message>
<xml_diff>
--- a/t/regression/xlsx_files/chart_bar01.xlsx
+++ b/t/regression/xlsx_files/chart_bar01.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" calcMode="autoNoTable"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -168,25 +168,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="64056320"/>
-        <c:axId val="64262912"/>
+        <c:axId val="64052224"/>
+        <c:axId val="64055552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="64056320"/>
+        <c:axId val="64052224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64262912"/>
+        <c:crossAx val="64055552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64262912"/>
+        <c:axId val="64055552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -194,7 +194,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64056320"/>
+        <c:crossAx val="64052224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>